<commit_message>
few updates for EU
</commit_message>
<xml_diff>
--- a/RawData/EU_RawData_VPython.xlsx
+++ b/RawData/EU_RawData_VPython.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\01_MFA_GlassIndustry\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1096A02-1A12-4E29-A450-B1FD2D7AA936}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA3A38E-FF46-4C8D-B0A9-E0B5B9A1A83D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="19650" windowHeight="13860" firstSheet="1" activeTab="4" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="19650" windowHeight="13860" activeTab="3" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
   </bookViews>
   <sheets>
     <sheet name="stock" sheetId="17" r:id="rId1"/>
     <sheet name="consumption" sheetId="16" r:id="rId2"/>
-    <sheet name="prod" sheetId="15" r:id="rId3"/>
+    <sheet name="prod" sheetId="20" r:id="rId3"/>
     <sheet name="import" sheetId="14" r:id="rId4"/>
     <sheet name="export" sheetId="12" r:id="rId5"/>
     <sheet name="workforce" sheetId="11" r:id="rId6"/>
@@ -56,7 +56,7 @@
             <family val="2"/>
           </rPr>
           <t>Unless otherwise indicated in a note attached to the cell, all data collected in this column comes from : 
-Ecodesign of Window Products. LOT 32, IfF, VHK and VITO, June 2015.</t>
+Ecodesign of Window Products. LOT 32, Task 3, IfF, VHK and VITO, June, 2015, p. 22</t>
         </r>
       </text>
     </comment>
@@ -163,7 +163,7 @@
     <author>jean</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{C2F8294C-B31F-43D8-B6AF-585789679304}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{F059D56F-DE8E-462B-B709-940839D868B5}">
       <text>
         <r>
           <rPr>
@@ -177,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{E278B976-4E5D-4CF3-857E-0C27846DEAE3}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{8FFAC56C-9F20-4C57-B69F-46C4751E7D08}">
       <text>
         <r>
           <rPr>
@@ -193,7 +193,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{50753E68-A245-4D7B-9CBE-A829F1613C3E}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{80DE692A-0D82-4ABD-BF2B-A0F9B0509919}">
       <text>
         <r>
           <rPr>
@@ -209,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{5A63D96A-0581-49AA-AF21-44B780879F75}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{BC044FF9-5242-4021-B857-18E0CF542688}">
       <text>
         <r>
           <rPr>
@@ -225,7 +225,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E27" authorId="0" shapeId="0" xr:uid="{AAB4A390-3B60-4C4E-B843-392CC59A122F}">
+    <comment ref="E27" authorId="0" shapeId="0" xr:uid="{2FFE3DD3-AC63-477C-AF0A-BB8559A6CCC5}">
       <text>
         <r>
           <rPr>
@@ -242,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E32" authorId="0" shapeId="0" xr:uid="{FB9EF9CB-05A2-474C-8923-74267D6DFFA7}">
+    <comment ref="E32" authorId="0" shapeId="0" xr:uid="{608AA8EB-5141-4B01-857A-BF5796CE27F1}">
       <text>
         <r>
           <rPr>
@@ -259,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D35" authorId="0" shapeId="0" xr:uid="{0E134010-E02E-4225-8906-789775788339}">
+    <comment ref="D35" authorId="0" shapeId="0" xr:uid="{2D00541E-5F06-4DE5-9E02-C6205EE8A6FA}">
       <text>
         <r>
           <rPr>
@@ -274,7 +274,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E38" authorId="0" shapeId="0" xr:uid="{F3B2E85C-31FC-406E-B6FD-895D5DAD64D7}">
+    <comment ref="E38" authorId="0" shapeId="0" xr:uid="{067A2B5D-1BD0-4D98-851E-39DACD586699}">
       <text>
         <r>
           <rPr>
@@ -291,7 +291,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D54" authorId="0" shapeId="0" xr:uid="{CBBF48C2-F469-4571-AC9E-684DE44CCF62}">
+    <comment ref="D54" authorId="0" shapeId="0" xr:uid="{1A5FC396-CA94-45D3-96D2-3CF51D654280}">
       <text>
         <r>
           <rPr>
@@ -304,7 +304,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C62" authorId="0" shapeId="0" xr:uid="{40DE4105-200D-4440-9B6B-6740067120DA}">
+    <comment ref="C62" authorId="0" shapeId="0" xr:uid="{61C0B995-E6D9-4B62-83E8-128177F7111C}">
       <text>
         <r>
           <rPr>
@@ -317,7 +317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C63" authorId="0" shapeId="0" xr:uid="{959CBDBD-EFD2-4543-91B8-75D3E697257E}">
+    <comment ref="C63" authorId="0" shapeId="0" xr:uid="{3420A8DA-86CD-461C-B5EF-E5E341F66904}">
       <text>
         <r>
           <rPr>
@@ -330,7 +330,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C64" authorId="0" shapeId="0" xr:uid="{9B416B7C-032F-4959-A6F7-232A6DCBAD31}">
+    <comment ref="C64" authorId="0" shapeId="0" xr:uid="{E2E6B502-5E11-486A-B7F5-F7D2D1A61F18}">
       <text>
         <r>
           <rPr>
@@ -343,7 +343,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C65" authorId="0" shapeId="0" xr:uid="{5654F17E-FD37-41F4-85BB-5CFE082C43A0}">
+    <comment ref="C65" authorId="0" shapeId="0" xr:uid="{ABA1165A-04A7-4E70-BB9B-891205CF7634}">
       <text>
         <r>
           <rPr>
@@ -356,7 +356,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C66" authorId="0" shapeId="0" xr:uid="{3235C2D9-908E-4084-8BA4-512AA9EE5E1C}">
+    <comment ref="C66" authorId="0" shapeId="0" xr:uid="{86F0C66A-9D33-4161-8B74-9A88C4258AD7}">
       <text>
         <r>
           <rPr>
@@ -369,7 +369,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C67" authorId="0" shapeId="0" xr:uid="{68B4C6D8-528F-4828-B32D-626BF8DEB7E5}">
+    <comment ref="C67" authorId="0" shapeId="0" xr:uid="{06079FF0-F391-474A-92DD-8AB76D15EB4C}">
       <text>
         <r>
           <rPr>
@@ -382,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C68" authorId="0" shapeId="0" xr:uid="{DC89D0C0-A259-4B07-8880-4343F538493F}">
+    <comment ref="C68" authorId="0" shapeId="0" xr:uid="{63DC345D-894D-4762-BAE5-B5F6842FA5D7}">
       <text>
         <r>
           <rPr>
@@ -395,7 +395,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C69" authorId="0" shapeId="0" xr:uid="{9CFD90AD-75AD-4C0B-8511-277A4CBF89F0}">
+    <comment ref="C69" authorId="0" shapeId="0" xr:uid="{7DC06089-8053-4DB1-A5ED-89B24AB09D0D}">
       <text>
         <r>
           <rPr>
@@ -408,7 +408,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C70" authorId="0" shapeId="0" xr:uid="{C01AC5BA-33CA-4ACC-9EFE-3057B9A863C2}">
+    <comment ref="C70" authorId="0" shapeId="0" xr:uid="{C54884A4-57A8-405A-AD39-2A87F9480410}">
       <text>
         <r>
           <rPr>
@@ -421,7 +421,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C71" authorId="0" shapeId="0" xr:uid="{435D93BD-7A36-4AED-B12A-DCC3FCF2054B}">
+    <comment ref="C71" authorId="0" shapeId="0" xr:uid="{16444560-60C6-4C97-80F2-6D350FD378B9}">
       <text>
         <r>
           <rPr>
@@ -434,7 +434,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C72" authorId="0" shapeId="0" xr:uid="{59AB2B1C-49AE-4FCE-9439-279E903197F7}">
+    <comment ref="C72" authorId="0" shapeId="0" xr:uid="{609C0CB6-A79E-4EC0-B78B-D9A591E2D528}">
       <text>
         <r>
           <rPr>
@@ -447,7 +447,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C73" authorId="0" shapeId="0" xr:uid="{5DDAD10A-A291-429B-9C03-53F481EF3719}">
+    <comment ref="C73" authorId="0" shapeId="0" xr:uid="{C2D64CB9-6768-4672-B9C2-D7DDC36BF91C}">
       <text>
         <r>
           <rPr>
@@ -460,7 +460,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C74" authorId="0" shapeId="0" xr:uid="{184CE6BF-C66C-4B8C-B844-AFCA8076D376}">
+    <comment ref="C74" authorId="0" shapeId="0" xr:uid="{7266362F-CE0F-4A8A-B31C-4BB1A3655F29}">
       <text>
         <r>
           <rPr>
@@ -473,7 +473,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C75" authorId="0" shapeId="0" xr:uid="{7B64207A-4B7F-49D4-8902-9CF4C4B55DD9}">
+    <comment ref="C75" authorId="0" shapeId="0" xr:uid="{1566FB03-5421-4053-856B-37728392DA6A}">
       <text>
         <r>
           <rPr>
@@ -486,7 +486,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C76" authorId="0" shapeId="0" xr:uid="{27841799-E6EF-4060-9FDB-24DBBDE88D1B}">
+    <comment ref="C76" authorId="0" shapeId="0" xr:uid="{04957374-FADF-46A2-A36D-5F0000E93D45}">
       <text>
         <r>
           <rPr>
@@ -499,7 +499,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C77" authorId="0" shapeId="0" xr:uid="{688390A4-8EB6-47A6-BDD3-34CFBF22EAD7}">
+    <comment ref="C77" authorId="0" shapeId="0" xr:uid="{AFC55CD5-7ABF-4C88-A904-6818D97FBE7D}">
       <text>
         <r>
           <rPr>
@@ -512,7 +512,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C78" authorId="0" shapeId="0" xr:uid="{D3E3CCD5-0CB8-4E7D-BB00-353131729589}">
+    <comment ref="C78" authorId="0" shapeId="0" xr:uid="{E3C9A90F-913A-4472-81F0-E7FCE402BC5C}">
       <text>
         <r>
           <rPr>
@@ -525,7 +525,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C79" authorId="0" shapeId="0" xr:uid="{2B8CC10E-D90B-4E24-B19A-923A89F556EB}">
+    <comment ref="C79" authorId="0" shapeId="0" xr:uid="{F84571EB-B01E-42E4-8975-7C5D1CF35C05}">
       <text>
         <r>
           <rPr>
@@ -538,7 +538,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C80" authorId="0" shapeId="0" xr:uid="{A4F9EAF2-1D64-4A10-AF7D-F515A422F0FA}">
+    <comment ref="C80" authorId="0" shapeId="0" xr:uid="{58526606-2914-4328-90D3-CB9AD6D547DF}">
       <text>
         <r>
           <rPr>
@@ -551,7 +551,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D80" authorId="0" shapeId="0" xr:uid="{EA54CD95-B976-4548-BA05-EFF0F9A21C82}">
+    <comment ref="D80" authorId="0" shapeId="0" xr:uid="{3090E952-025D-4482-89E6-80FD7B080CB1}">
       <text>
         <r>
           <rPr>
@@ -565,7 +565,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C81" authorId="0" shapeId="0" xr:uid="{B9929390-98CF-4C9B-8E80-FE30A5F81702}">
+    <comment ref="C81" authorId="0" shapeId="0" xr:uid="{AE1B76E1-63E4-4BE0-A1EC-B4D9B663AEBD}">
       <text>
         <r>
           <rPr>
@@ -1846,7 +1846,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
   <si>
     <t>year</t>
   </si>
@@ -1864,9 +1864,6 @@
   </si>
   <si>
     <t>non-residential glazing, "000 m²</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>glass ind., unit</t>
@@ -2587,7 +2584,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2715,7 +2712,6 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -2726,7 +2722,6 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -2737,7 +2732,6 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -2748,7 +2742,6 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -2759,7 +2752,6 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
     </row>
     <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -2788,9 +2780,6 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="12" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="14" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -2801,9 +2790,6 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="12"/>
-      <c r="E14" s="12" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="15" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -2814,7 +2800,6 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -2825,7 +2810,6 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
     </row>
     <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -2836,7 +2820,6 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -2847,7 +2830,6 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
     </row>
     <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -2858,7 +2840,6 @@
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -2869,7 +2850,6 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
     </row>
     <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
@@ -2880,7 +2860,6 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
     </row>
     <row r="22" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
@@ -2909,7 +2888,6 @@
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
     </row>
     <row r="24" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
@@ -2920,7 +2898,6 @@
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
     </row>
     <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
@@ -2931,7 +2908,6 @@
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
     </row>
     <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
@@ -2942,7 +2918,6 @@
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
     </row>
     <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
@@ -2953,7 +2928,6 @@
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
     </row>
     <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
@@ -2964,7 +2938,6 @@
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
     </row>
     <row r="29" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
@@ -2975,7 +2948,6 @@
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
     </row>
     <row r="30" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
@@ -2986,7 +2958,6 @@
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
     </row>
     <row r="31" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
@@ -2997,7 +2968,6 @@
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
     </row>
     <row r="32" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
@@ -3026,7 +2996,6 @@
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
     </row>
     <row r="34" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
@@ -3037,9 +3006,6 @@
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="12"/>
-      <c r="E34" s="12" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="35" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
@@ -3050,7 +3016,6 @@
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
     </row>
     <row r="36" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
@@ -3061,7 +3026,6 @@
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
     </row>
     <row r="37" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
@@ -3072,7 +3036,6 @@
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
     </row>
     <row r="38" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
@@ -3083,7 +3046,6 @@
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
     </row>
     <row r="39" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
@@ -3094,7 +3056,6 @@
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
     </row>
     <row r="40" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
@@ -3105,7 +3066,6 @@
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
     </row>
     <row r="41" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
@@ -3116,7 +3076,6 @@
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
     </row>
     <row r="42" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
@@ -3145,7 +3104,6 @@
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
     </row>
     <row r="44" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
@@ -3156,7 +3114,6 @@
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
     </row>
     <row r="45" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
@@ -3167,7 +3124,6 @@
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
     </row>
     <row r="46" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
@@ -3178,7 +3134,6 @@
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
     </row>
     <row r="47" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
@@ -3189,7 +3144,6 @@
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
     </row>
     <row r="48" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
@@ -3200,7 +3154,6 @@
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
     </row>
     <row r="49" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
@@ -3211,7 +3164,6 @@
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
     </row>
     <row r="50" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
@@ -3222,7 +3174,6 @@
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
     </row>
     <row r="51" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
@@ -3233,7 +3184,6 @@
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
     </row>
     <row r="52" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
@@ -3262,7 +3212,6 @@
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
     </row>
     <row r="54" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
@@ -3273,7 +3222,6 @@
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
     </row>
     <row r="55" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
@@ -3284,7 +3232,6 @@
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
     </row>
     <row r="56" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
@@ -3295,7 +3242,6 @@
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
     </row>
     <row r="57" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
@@ -3306,7 +3252,6 @@
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
     </row>
     <row r="58" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
@@ -3317,7 +3262,6 @@
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
     </row>
     <row r="59" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
@@ -3328,7 +3272,6 @@
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
     </row>
     <row r="60" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
@@ -3339,7 +3282,6 @@
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
     </row>
     <row r="61" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
@@ -3350,7 +3292,6 @@
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
     </row>
     <row r="62" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
@@ -3379,7 +3320,6 @@
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
     </row>
     <row r="64" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
@@ -3390,7 +3330,6 @@
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="12"/>
-      <c r="E64" s="12"/>
     </row>
     <row r="65" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
@@ -3404,7 +3343,6 @@
         <v>4927680</v>
       </c>
       <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
     </row>
     <row r="66" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
@@ -3415,7 +3353,6 @@
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
     </row>
     <row r="67" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
@@ -3426,7 +3363,6 @@
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="12"/>
-      <c r="E67" s="12"/>
     </row>
     <row r="68" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
@@ -3437,7 +3373,6 @@
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
     </row>
     <row r="69" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
@@ -3448,7 +3383,6 @@
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="12"/>
-      <c r="E69" s="12"/>
     </row>
     <row r="70" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
@@ -3459,7 +3393,6 @@
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="12"/>
-      <c r="E70" s="12"/>
     </row>
     <row r="71" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
@@ -3470,7 +3403,6 @@
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="12"/>
-      <c r="E71" s="12"/>
     </row>
     <row r="72" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
@@ -3981,7 +3913,7 @@
   <dimension ref="A1:BS93"/>
   <sheetViews>
     <sheetView zoomScale="65" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
@@ -4005,13 +3937,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="46" t="s">
         <v>17</v>
-      </c>
-      <c r="D1" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="46" t="s">
-        <v>18</v>
       </c>
       <c r="F1" s="46" t="s">
         <v>1</v>
@@ -5420,14 +5352,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984B49BA-6D54-42C1-84EE-7F8663080B50}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D014A44-A0D2-41E4-AD5D-2CB29E224E01}">
   <dimension ref="A1:BT105"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B62" sqref="B62"/>
+      <selection pane="bottomRight" activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5451,16 +5383,16 @@
         <v>3</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -7828,11 +7760,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B1BC36-79CC-403E-BDAB-F4ACF4DC04E2}">
   <dimension ref="A1:BT100"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C69" sqref="C69"/>
+      <selection pane="bottomRight" activeCell="M85" sqref="M85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7855,19 +7787,19 @@
         <v>3</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="F1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8915,7 +8847,7 @@
         <v>2012</v>
       </c>
       <c r="C77" s="3">
-        <f>E77+D77</f>
+        <f t="shared" ref="C77:C83" si="1">E77+D77</f>
         <v>1004.049</v>
       </c>
       <c r="D77" s="3">
@@ -8943,7 +8875,7 @@
         <v>2013</v>
       </c>
       <c r="C78" s="3">
-        <f>E78+D78</f>
+        <f t="shared" si="1"/>
         <v>946.01599999999996</v>
       </c>
       <c r="D78" s="3">
@@ -8971,7 +8903,7 @@
         <v>2014</v>
       </c>
       <c r="C79" s="3">
-        <f>E79+D79</f>
+        <f t="shared" si="1"/>
         <v>1034.6280000000002</v>
       </c>
       <c r="D79" s="3">
@@ -8999,7 +8931,7 @@
         <v>2015</v>
       </c>
       <c r="C80" s="3">
-        <f>E80+D80</f>
+        <f t="shared" si="1"/>
         <v>1079.1000000000001</v>
       </c>
       <c r="D80" s="3">
@@ -9027,7 +8959,7 @@
         <v>2016</v>
       </c>
       <c r="C81" s="3">
-        <f>E81+D81</f>
+        <f t="shared" si="1"/>
         <v>1255.011</v>
       </c>
       <c r="D81" s="3">
@@ -9054,7 +8986,7 @@
         <v>2017</v>
       </c>
       <c r="C82" s="3">
-        <f>E82+D82</f>
+        <f t="shared" si="1"/>
         <v>1534.989</v>
       </c>
       <c r="D82" s="3">
@@ -9081,7 +9013,7 @@
         <v>2018</v>
       </c>
       <c r="C83" s="3">
-        <f>E83+D83</f>
+        <f t="shared" si="1"/>
         <v>1673.6289999999999</v>
       </c>
       <c r="D83" s="3">
@@ -9514,11 +9446,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2629125-5F59-4D2B-B790-D44D45AA199C}">
   <dimension ref="A1:BU102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G37" sqref="G37"/>
+      <selection pane="bottomRight" activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9540,19 +9472,19 @@
         <v>3</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="F1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -11226,13 +11158,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -12461,67 +12393,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="G1" s="35"/>
       <c r="H1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="M1" s="35"/>
       <c r="N1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="S1" s="35"/>
       <c r="T1" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="V1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -14037,10 +13969,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -15471,22 +15403,22 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update of the notebook taking into account multiindexing, problem with small multiples in seaborn
</commit_message>
<xml_diff>
--- a/RawData/EU_RawData_VPython.xlsx
+++ b/RawData/EU_RawData_VPython.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\01_MFA_GlassIndustry\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA3A38E-FF46-4C8D-B0A9-E0B5B9A1A83D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F8B956-D0F2-4EAE-9E33-87B221E3B769}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="19650" windowHeight="13860" activeTab="3" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
+    <workbookView xWindow="3900" yWindow="1530" windowWidth="21510" windowHeight="14670" firstSheet="1" activeTab="6" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
   </bookViews>
   <sheets>
     <sheet name="stock" sheetId="17" r:id="rId1"/>
@@ -1416,7 +1416,7 @@
     <author>jean</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{2218B88B-1E8A-40E1-872F-DDB6B93A82C7}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{C2855AB6-36CF-44AB-88D5-53E4AAFFC284}">
       <text>
         <r>
           <rPr>
@@ -1430,7 +1430,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{0B8DCAF5-6651-4811-A2B6-D192113267D7}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{2218B88B-1E8A-40E1-872F-DDB6B93A82C7}">
       <text>
         <r>
           <rPr>
@@ -1444,7 +1444,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{DEBD7CA6-B32A-49EF-BCEE-33043A999820}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{0B8DCAF5-6651-4811-A2B6-D192113267D7}">
       <text>
         <r>
           <rPr>
@@ -1458,7 +1458,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{397224C5-0620-4957-8D24-5AE18E44D756}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{DEBD7CA6-B32A-49EF-BCEE-33043A999820}">
       <text>
         <r>
           <rPr>
@@ -1472,7 +1472,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{062A2D02-1513-4DE1-9436-E1315FFB4693}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{397224C5-0620-4957-8D24-5AE18E44D756}">
       <text>
         <r>
           <rPr>
@@ -1486,7 +1486,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{ABBF27CE-AB17-4B62-821A-DD0067859E7A}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{062A2D02-1513-4DE1-9436-E1315FFB4693}">
       <text>
         <r>
           <rPr>
@@ -1500,7 +1500,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{F0275E9E-AE0E-4978-8287-4440143E8699}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{ABBF27CE-AB17-4B62-821A-DD0067859E7A}">
       <text>
         <r>
           <rPr>
@@ -1514,7 +1514,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{720C057B-9594-4FEA-B206-AF2D2A88B8B5}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{F0275E9E-AE0E-4978-8287-4440143E8699}">
       <text>
         <r>
           <rPr>
@@ -1528,7 +1528,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{451737A2-687A-4FEA-BD0E-7148A1A16F52}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{720C057B-9594-4FEA-B206-AF2D2A88B8B5}">
       <text>
         <r>
           <rPr>
@@ -1542,7 +1542,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{1262E888-F996-4D4B-AAD7-67035BFF41BF}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{451737A2-687A-4FEA-BD0E-7148A1A16F52}">
       <text>
         <r>
           <rPr>
@@ -1556,7 +1556,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{0A7FF325-4795-4709-B14E-12ECB9286D83}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{1262E888-F996-4D4B-AAD7-67035BFF41BF}">
       <text>
         <r>
           <rPr>
@@ -1570,7 +1570,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{0C600EC5-2816-4118-84DE-CEBA05D52076}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{0A7FF325-4795-4709-B14E-12ECB9286D83}">
       <text>
         <r>
           <rPr>
@@ -1584,7 +1584,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{BEE0B9C3-B1EA-4159-A420-D745E657DC38}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{0C600EC5-2816-4118-84DE-CEBA05D52076}">
       <text>
         <r>
           <rPr>
@@ -1598,7 +1598,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{40CBC84D-4932-4800-AE6E-9D9600F536EF}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{BEE0B9C3-B1EA-4159-A420-D745E657DC38}">
       <text>
         <r>
           <rPr>
@@ -1612,7 +1612,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{E4CD590C-D6AE-40A7-8364-C1C587FA3E12}">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{40CBC84D-4932-4800-AE6E-9D9600F536EF}">
       <text>
         <r>
           <rPr>
@@ -1626,7 +1626,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{46A0FBBA-2F34-4AD0-A428-A29EA8001325}">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{E4CD590C-D6AE-40A7-8364-C1C587FA3E12}">
       <text>
         <r>
           <rPr>
@@ -1640,7 +1640,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{C90EA2CB-7B80-4E07-8E6A-2E7EF1F64E0B}">
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{46A0FBBA-2F34-4AD0-A428-A29EA8001325}">
       <text>
         <r>
           <rPr>
@@ -1654,7 +1654,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{39293397-21C8-4D7D-A801-C41F3BCFC47C}">
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{C90EA2CB-7B80-4E07-8E6A-2E7EF1F64E0B}">
       <text>
         <r>
           <rPr>
@@ -1668,7 +1668,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{E66E9267-CC37-4EAF-AB1C-F2FD4D32244B}">
+    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{39293397-21C8-4D7D-A801-C41F3BCFC47C}">
       <text>
         <r>
           <rPr>
@@ -1682,7 +1682,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{9308057F-C550-4744-8060-39B074F9BFB2}">
+    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{E66E9267-CC37-4EAF-AB1C-F2FD4D32244B}">
       <text>
         <r>
           <rPr>
@@ -1693,6 +1693,61 @@
           </rPr>
           <t>Unless otherwise indicated in a note attached to the cell, all data collected in this column comes from:
 The glass industry in the European Economic Community, Commission of the European Communities, 1984</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{9308057F-C550-4744-8060-39B074F9BFB2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unless otherwise indicated in a note attached to the cell, all data collected in this column comes from:
+The glass industry in the European Economic Community, Commission of the European Communities, 1984</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{27BF96C4-1918-4424-AF42-DE3DD4B7885D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Boaglio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{7404C297-C888-4CDB-8837-12939F2F6D10}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Plan d’action sectoriel visant a l’amelioration de l’efficience energetique a l’horizon 2012 dans l’industrie verriere en wallonie</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B68" authorId="0" shapeId="0" xr:uid="{64676118-BB2E-4054-86E7-4A8894595376}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Life Cycle Assessment of Float Glass, PE International, 2011
+https://glassforeurope.com/report-life-cycle-assessment-of-float-glass/
+(accessed September 30, 2020)</t>
         </r>
       </text>
     </comment>
@@ -1846,7 +1901,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -1984,6 +2039,9 @@
   </si>
   <si>
     <t>flat glass (processed), kt</t>
+  </si>
+  <si>
+    <t>Specific consumption, GJ/t</t>
   </si>
 </sst>
 </file>
@@ -2123,7 +2181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2263,6 +2321,18 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2581,10 +2651,10 @@
   <dimension ref="A1:BT93"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomRight" activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3913,7 +3983,7 @@
   <dimension ref="A1:BS93"/>
   <sheetViews>
     <sheetView zoomScale="65" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
@@ -5355,11 +5425,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D014A44-A0D2-41E4-AD5D-2CB29E224E01}">
   <dimension ref="A1:BT105"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E86" sqref="E86"/>
+      <selection pane="bottomRight" activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7760,8 +7830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B1BC36-79CC-403E-BDAB-F4ACF4DC04E2}">
   <dimension ref="A1:BT100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="M85" sqref="M85"/>
@@ -11137,7 +11207,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12364,203 +12434,215 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46AF0D7-F026-4606-8FE3-F48C9C7C976D}">
-  <dimension ref="A1:BV76"/>
+  <dimension ref="A1:BX76"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="7" customWidth="1"/>
-    <col min="4" max="6" width="21.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="4.5703125" style="36" customWidth="1"/>
-    <col min="8" max="12" width="21.140625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="4.5703125" style="36" customWidth="1"/>
-    <col min="14" max="18" width="21.140625" style="6" customWidth="1"/>
-    <col min="19" max="19" width="4.42578125" style="36" customWidth="1"/>
-    <col min="20" max="24" width="21.140625" style="6" customWidth="1"/>
-    <col min="25" max="16384" width="10.7109375" style="6"/>
+    <col min="2" max="2" width="13.5703125" style="53" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" style="36" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="7" customWidth="1"/>
+    <col min="6" max="8" width="21.140625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" style="36" customWidth="1"/>
+    <col min="10" max="14" width="21.140625" style="6" customWidth="1"/>
+    <col min="15" max="15" width="4.5703125" style="36" customWidth="1"/>
+    <col min="16" max="20" width="21.140625" style="6" customWidth="1"/>
+    <col min="21" max="21" width="4.42578125" style="36" customWidth="1"/>
+    <col min="22" max="26" width="21.140625" style="6" customWidth="1"/>
+    <col min="27" max="16384" width="10.7109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="35"/>
+      <c r="D1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="35"/>
+      <c r="J1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="35"/>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="35"/>
+      <c r="P1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="S1" s="35"/>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="35"/>
+      <c r="V1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>1945</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>1946</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>1947</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B4" s="51">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>1948</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>1949</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>1950</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>1951</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>1952</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>1953</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>1954</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>1955</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B12" s="54">
+        <v>35</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>1956</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>1957</v>
       </c>
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>1958</v>
       </c>
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>1959</v>
       </c>
-      <c r="C16" s="8"/>
-    </row>
-    <row r="17" spans="1:74" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:76" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>1960</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="8"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="36"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="8"/>
+      <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="I17" s="36"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
-      <c r="M17" s="36"/>
+      <c r="M17" s="6"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
+      <c r="O17" s="36"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
-      <c r="S17" s="36"/>
+      <c r="S17" s="6"/>
       <c r="T17" s="6"/>
-      <c r="U17" s="6"/>
+      <c r="U17" s="36"/>
       <c r="V17" s="6"/>
       <c r="W17" s="6"/>
       <c r="X17" s="6"/>
@@ -12614,30 +12696,32 @@
       <c r="BT17" s="6"/>
       <c r="BU17" s="6"/>
       <c r="BV17" s="6"/>
-    </row>
-    <row r="18" spans="1:74" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BW17" s="6"/>
+      <c r="BX17" s="6"/>
+    </row>
+    <row r="18" spans="1:76" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>1961</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="8"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="36"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="8"/>
+      <c r="G18" s="6"/>
       <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
+      <c r="I18" s="36"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
-      <c r="M18" s="36"/>
+      <c r="M18" s="6"/>
       <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
+      <c r="O18" s="36"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
-      <c r="S18" s="36"/>
+      <c r="S18" s="6"/>
       <c r="T18" s="6"/>
-      <c r="U18" s="6"/>
+      <c r="U18" s="36"/>
       <c r="V18" s="6"/>
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
@@ -12691,30 +12775,32 @@
       <c r="BT18" s="6"/>
       <c r="BU18" s="6"/>
       <c r="BV18" s="6"/>
-    </row>
-    <row r="19" spans="1:74" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BW18" s="6"/>
+      <c r="BX18" s="6"/>
+    </row>
+    <row r="19" spans="1:76" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>1962</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="8"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="36"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="8"/>
+      <c r="G19" s="6"/>
       <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="I19" s="36"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
-      <c r="M19" s="36"/>
+      <c r="M19" s="6"/>
       <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
+      <c r="O19" s="36"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
-      <c r="S19" s="36"/>
+      <c r="S19" s="6"/>
       <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
+      <c r="U19" s="36"/>
       <c r="V19" s="6"/>
       <c r="W19" s="6"/>
       <c r="X19" s="6"/>
@@ -12768,61 +12854,63 @@
       <c r="BT19" s="6"/>
       <c r="BU19" s="6"/>
       <c r="BV19" s="6"/>
-    </row>
-    <row r="20" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="BW19" s="6"/>
+      <c r="BX19" s="6"/>
+    </row>
+    <row r="20" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>1963</v>
       </c>
     </row>
-    <row r="21" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>1964</v>
       </c>
     </row>
-    <row r="22" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>1965</v>
       </c>
     </row>
-    <row r="23" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>1966</v>
       </c>
     </row>
-    <row r="24" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>1967</v>
       </c>
     </row>
-    <row r="25" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>1968</v>
       </c>
     </row>
-    <row r="26" spans="1:74" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:76" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>1969</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="36"/>
+      <c r="G26" s="6"/>
       <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
+      <c r="I26" s="36"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
-      <c r="M26" s="36"/>
+      <c r="M26" s="6"/>
       <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
+      <c r="O26" s="36"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
-      <c r="S26" s="36"/>
+      <c r="S26" s="6"/>
       <c r="T26" s="6"/>
-      <c r="U26" s="6"/>
+      <c r="U26" s="36"/>
       <c r="V26" s="6"/>
       <c r="W26" s="6"/>
       <c r="X26" s="6"/>
@@ -12876,76 +12964,80 @@
       <c r="BT26" s="6"/>
       <c r="BU26" s="6"/>
       <c r="BV26" s="6"/>
-    </row>
-    <row r="27" spans="1:74" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BW26" s="6"/>
+      <c r="BX26" s="6"/>
+    </row>
+    <row r="27" spans="1:76" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>1970</v>
       </c>
-      <c r="B27" s="37">
+      <c r="B27" s="53">
+        <v>17.5</v>
+      </c>
+      <c r="C27" s="40"/>
+      <c r="D27" s="37">
         <v>27.611000000000001</v>
       </c>
-      <c r="C27" s="38">
+      <c r="E27" s="38">
         <v>78.8</v>
       </c>
-      <c r="D27" s="39">
+      <c r="F27" s="39">
         <v>17</v>
       </c>
-      <c r="E27" s="39">
+      <c r="G27" s="39">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F27" s="39">
+      <c r="H27" s="39">
         <v>0</v>
       </c>
-      <c r="G27" s="40"/>
-      <c r="H27" s="39">
+      <c r="I27" s="40"/>
+      <c r="J27" s="39">
         <v>10.363</v>
       </c>
-      <c r="I27" s="39">
+      <c r="K27" s="39">
         <v>78.5</v>
       </c>
-      <c r="J27" s="39">
+      <c r="L27" s="39">
         <v>14.4</v>
       </c>
-      <c r="K27" s="39">
+      <c r="M27" s="39">
         <v>7.1</v>
       </c>
-      <c r="L27" s="39">
+      <c r="N27" s="39">
         <v>0</v>
       </c>
-      <c r="M27" s="40"/>
-      <c r="N27" s="39">
+      <c r="O27" s="40"/>
+      <c r="P27" s="39">
         <v>10.976000000000001</v>
       </c>
-      <c r="O27" s="39">
+      <c r="Q27" s="39">
         <v>66.7</v>
       </c>
-      <c r="P27" s="39">
+      <c r="R27" s="39">
         <v>26.8</v>
       </c>
-      <c r="Q27" s="39">
+      <c r="S27" s="39">
         <v>6.4</v>
       </c>
-      <c r="R27" s="39">
+      <c r="T27" s="39">
         <v>0.1</v>
       </c>
-      <c r="S27" s="40"/>
-      <c r="T27" s="39">
+      <c r="U27" s="40"/>
+      <c r="V27" s="39">
         <v>10.3</v>
       </c>
-      <c r="U27" s="39">
+      <c r="W27" s="39">
         <v>74.400000000000006</v>
       </c>
-      <c r="V27" s="39">
+      <c r="X27" s="39">
         <v>9.6999999999999993</v>
       </c>
-      <c r="W27" s="39">
+      <c r="Y27" s="39">
         <v>6.4</v>
       </c>
-      <c r="X27" s="39">
+      <c r="Z27" s="39">
         <v>9.5</v>
       </c>
-      <c r="Y27" s="6"/>
-      <c r="Z27" s="6"/>
       <c r="AA27" s="6"/>
       <c r="AB27" s="6"/>
       <c r="AC27" s="6"/>
@@ -12994,801 +13086,838 @@
       <c r="BT27" s="6"/>
       <c r="BU27" s="6"/>
       <c r="BV27" s="6"/>
-    </row>
-    <row r="28" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="BW27" s="6"/>
+      <c r="BX27" s="6"/>
+    </row>
+    <row r="28" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>1971</v>
       </c>
-      <c r="B28" s="37">
+      <c r="C28" s="40"/>
+      <c r="D28" s="37">
         <v>27.611000000000001</v>
       </c>
-      <c r="C28" s="38">
+      <c r="E28" s="38">
         <v>78.8</v>
       </c>
-      <c r="D28" s="39">
+      <c r="F28" s="39">
         <v>17</v>
       </c>
-      <c r="E28" s="39">
+      <c r="G28" s="39">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F28" s="39">
+      <c r="H28" s="39">
         <v>0</v>
       </c>
-      <c r="G28" s="40"/>
-      <c r="H28" s="39">
+      <c r="I28" s="40"/>
+      <c r="J28" s="39">
         <v>10.363</v>
       </c>
-      <c r="I28" s="39">
+      <c r="K28" s="39">
         <v>78.5</v>
       </c>
-      <c r="J28" s="39">
+      <c r="L28" s="39">
         <v>14.4</v>
       </c>
-      <c r="K28" s="39">
+      <c r="M28" s="39">
         <v>7.1</v>
       </c>
-      <c r="L28" s="39">
+      <c r="N28" s="39">
         <v>0</v>
       </c>
-      <c r="M28" s="40"/>
-      <c r="N28" s="39">
+      <c r="O28" s="40"/>
+      <c r="P28" s="39">
         <v>10.976000000000001</v>
       </c>
-      <c r="O28" s="39">
+      <c r="Q28" s="39">
         <v>66.7</v>
       </c>
-      <c r="P28" s="39">
+      <c r="R28" s="39">
         <v>26.8</v>
       </c>
-      <c r="Q28" s="39">
+      <c r="S28" s="39">
         <v>6.4</v>
       </c>
-      <c r="R28" s="39">
+      <c r="T28" s="39">
         <v>0.1</v>
       </c>
-      <c r="S28" s="40"/>
-      <c r="T28" s="39">
+      <c r="U28" s="40"/>
+      <c r="V28" s="39">
         <v>10.3</v>
       </c>
-      <c r="U28" s="39">
+      <c r="W28" s="39">
         <v>74.400000000000006</v>
       </c>
-      <c r="V28" s="39">
+      <c r="X28" s="39">
         <v>9.6999999999999993</v>
       </c>
-      <c r="W28" s="39">
+      <c r="Y28" s="39">
         <v>6.4</v>
       </c>
-      <c r="X28" s="39">
+      <c r="Z28" s="39">
         <v>9.5</v>
       </c>
     </row>
-    <row r="29" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>1972</v>
       </c>
-      <c r="B29" s="37">
+      <c r="C29" s="40"/>
+      <c r="D29" s="37">
         <v>27.611000000000001</v>
       </c>
-      <c r="C29" s="38">
+      <c r="E29" s="38">
         <v>78.8</v>
       </c>
-      <c r="D29" s="39">
+      <c r="F29" s="39">
         <v>17</v>
       </c>
-      <c r="E29" s="39">
+      <c r="G29" s="39">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F29" s="39">
+      <c r="H29" s="39">
         <v>0</v>
       </c>
-      <c r="G29" s="40"/>
-      <c r="H29" s="39">
+      <c r="I29" s="40"/>
+      <c r="J29" s="39">
         <v>10.363</v>
       </c>
-      <c r="I29" s="39">
+      <c r="K29" s="39">
         <v>78.5</v>
       </c>
-      <c r="J29" s="39">
+      <c r="L29" s="39">
         <v>14.4</v>
       </c>
-      <c r="K29" s="39">
+      <c r="M29" s="39">
         <v>7.1</v>
       </c>
-      <c r="L29" s="39">
+      <c r="N29" s="39">
         <v>0</v>
       </c>
-      <c r="M29" s="40"/>
-      <c r="N29" s="39">
+      <c r="O29" s="40"/>
+      <c r="P29" s="39">
         <v>10.976000000000001</v>
       </c>
-      <c r="O29" s="39">
+      <c r="Q29" s="39">
         <v>66.7</v>
       </c>
-      <c r="P29" s="39">
+      <c r="R29" s="39">
         <v>26.8</v>
       </c>
-      <c r="Q29" s="39">
+      <c r="S29" s="39">
         <v>6.4</v>
       </c>
-      <c r="R29" s="39">
+      <c r="T29" s="39">
         <v>0.1</v>
       </c>
-      <c r="S29" s="40"/>
-      <c r="T29" s="39">
+      <c r="U29" s="40"/>
+      <c r="V29" s="39">
         <v>10.3</v>
       </c>
-      <c r="U29" s="39">
+      <c r="W29" s="39">
         <v>74.400000000000006</v>
       </c>
-      <c r="V29" s="39">
+      <c r="X29" s="39">
         <v>9.6999999999999993</v>
       </c>
-      <c r="W29" s="39">
+      <c r="Y29" s="39">
         <v>6.4</v>
       </c>
-      <c r="X29" s="39">
+      <c r="Z29" s="39">
         <v>9.5</v>
       </c>
     </row>
-    <row r="30" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>1973</v>
       </c>
-      <c r="B30" s="37">
+      <c r="C30" s="40"/>
+      <c r="D30" s="37">
         <v>27.611000000000001</v>
       </c>
-      <c r="C30" s="38">
+      <c r="E30" s="38">
         <v>78.900000000000006</v>
       </c>
-      <c r="D30" s="39">
+      <c r="F30" s="39">
         <v>17</v>
       </c>
-      <c r="E30" s="39">
+      <c r="G30" s="39">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F30" s="39">
+      <c r="H30" s="39">
         <v>0</v>
       </c>
-      <c r="G30" s="40"/>
-      <c r="H30" s="39">
+      <c r="I30" s="40"/>
+      <c r="J30" s="39">
         <v>10.363</v>
       </c>
-      <c r="I30" s="39">
+      <c r="K30" s="39">
         <v>78.5</v>
       </c>
-      <c r="J30" s="39">
+      <c r="L30" s="39">
         <v>14.4</v>
       </c>
-      <c r="K30" s="39">
+      <c r="M30" s="39">
         <v>7.1</v>
       </c>
-      <c r="L30" s="39">
+      <c r="N30" s="39">
         <v>0</v>
       </c>
-      <c r="M30" s="40"/>
-      <c r="N30" s="39">
+      <c r="O30" s="40"/>
+      <c r="P30" s="39">
         <v>10.976000000000001</v>
       </c>
-      <c r="O30" s="39">
+      <c r="Q30" s="39">
         <v>66.7</v>
       </c>
-      <c r="P30" s="39">
+      <c r="R30" s="39">
         <v>26.8</v>
       </c>
-      <c r="Q30" s="39">
+      <c r="S30" s="39">
         <v>6.4</v>
       </c>
-      <c r="R30" s="39">
+      <c r="T30" s="39">
         <v>0.1</v>
       </c>
-      <c r="S30" s="40"/>
-      <c r="T30" s="39">
+      <c r="U30" s="40"/>
+      <c r="V30" s="39">
         <v>10.3</v>
       </c>
-      <c r="U30" s="39">
+      <c r="W30" s="39">
         <v>74.400000000000006</v>
       </c>
-      <c r="V30" s="39">
+      <c r="X30" s="39">
         <v>9.6999999999999993</v>
       </c>
-      <c r="W30" s="39">
+      <c r="Y30" s="39">
         <v>6.4</v>
       </c>
-      <c r="X30" s="39">
+      <c r="Z30" s="39">
         <v>9.5</v>
       </c>
     </row>
-    <row r="31" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>1974</v>
       </c>
-      <c r="B31" s="37">
+      <c r="B31" s="53">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="C31" s="40"/>
+      <c r="D31" s="37">
         <v>27.609000000000002</v>
       </c>
-      <c r="C31" s="38">
+      <c r="E31" s="38">
         <v>80.400000000000006</v>
       </c>
-      <c r="D31" s="39">
+      <c r="F31" s="39">
         <v>15.4</v>
       </c>
-      <c r="E31" s="39">
+      <c r="G31" s="39">
         <v>4.2</v>
       </c>
-      <c r="F31" s="39">
+      <c r="H31" s="39">
         <v>0</v>
       </c>
-      <c r="G31" s="40"/>
-      <c r="H31" s="39">
+      <c r="I31" s="40"/>
+      <c r="J31" s="39">
         <v>10.863</v>
       </c>
-      <c r="I31" s="39">
+      <c r="K31" s="39">
         <v>66.5</v>
       </c>
-      <c r="J31" s="39">
+      <c r="L31" s="39">
         <v>27.2</v>
       </c>
-      <c r="K31" s="39">
+      <c r="M31" s="39">
         <v>6.3</v>
       </c>
-      <c r="L31" s="39">
+      <c r="N31" s="39">
         <v>0</v>
       </c>
-      <c r="M31" s="40"/>
-      <c r="N31" s="39">
+      <c r="O31" s="40"/>
+      <c r="P31" s="39">
         <v>9.4339999999999993</v>
       </c>
-      <c r="O31" s="39">
+      <c r="Q31" s="39">
         <v>62</v>
       </c>
-      <c r="P31" s="39">
+      <c r="R31" s="39">
         <v>30.8</v>
       </c>
-      <c r="Q31" s="39">
+      <c r="S31" s="39">
         <v>7.2</v>
       </c>
-      <c r="R31" s="39">
+      <c r="T31" s="39">
         <v>0</v>
       </c>
-      <c r="S31" s="40"/>
-      <c r="T31" s="39">
+      <c r="U31" s="40"/>
+      <c r="V31" s="39">
         <v>9.7530000000000001</v>
       </c>
-      <c r="U31" s="39">
+      <c r="W31" s="39">
         <v>69.900000000000006</v>
       </c>
-      <c r="V31" s="39">
+      <c r="X31" s="39">
         <v>14.4</v>
       </c>
-      <c r="W31" s="39">
+      <c r="Y31" s="39">
         <v>5.7</v>
       </c>
-      <c r="X31" s="39">
+      <c r="Z31" s="39">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>1975</v>
       </c>
-      <c r="B32" s="37">
+      <c r="B32" s="53">
+        <v>16.7</v>
+      </c>
+      <c r="C32" s="40"/>
+      <c r="D32" s="37">
         <v>21.454999999999998</v>
       </c>
-      <c r="C32" s="38">
+      <c r="E32" s="38">
         <v>76.5</v>
       </c>
-      <c r="D32" s="39">
+      <c r="F32" s="39">
         <v>19</v>
       </c>
-      <c r="E32" s="39">
+      <c r="G32" s="39">
         <v>4.5</v>
       </c>
-      <c r="F32" s="39">
+      <c r="H32" s="39">
         <v>0</v>
       </c>
-      <c r="G32" s="40"/>
-      <c r="H32" s="39">
+      <c r="I32" s="40"/>
+      <c r="J32" s="39">
         <v>8.8529999999999998</v>
       </c>
-      <c r="I32" s="39">
+      <c r="K32" s="39">
         <v>61.8</v>
       </c>
-      <c r="J32" s="39">
+      <c r="L32" s="39">
         <v>30.7</v>
       </c>
-      <c r="K32" s="39">
+      <c r="M32" s="39">
         <v>7.5</v>
       </c>
-      <c r="L32" s="39">
+      <c r="N32" s="39">
         <v>0</v>
       </c>
-      <c r="M32" s="40"/>
-      <c r="N32" s="39">
+      <c r="O32" s="40"/>
+      <c r="P32" s="39">
         <v>9.1509999999999998</v>
       </c>
-      <c r="O32" s="39">
+      <c r="Q32" s="39">
         <v>60.3</v>
       </c>
-      <c r="P32" s="39">
+      <c r="R32" s="39">
         <v>31.6</v>
       </c>
-      <c r="Q32" s="39">
+      <c r="S32" s="39">
         <v>8.1</v>
       </c>
-      <c r="R32" s="39">
+      <c r="T32" s="39">
         <v>0</v>
       </c>
-      <c r="S32" s="40"/>
-      <c r="T32" s="39">
+      <c r="U32" s="40"/>
+      <c r="V32" s="39">
         <v>8.4689999999999994</v>
       </c>
-      <c r="U32" s="39">
+      <c r="W32" s="39">
         <v>67</v>
       </c>
-      <c r="V32" s="39">
+      <c r="X32" s="39">
         <v>16.100000000000001</v>
       </c>
-      <c r="W32" s="39">
+      <c r="Y32" s="39">
         <v>5.4</v>
       </c>
-      <c r="X32" s="39">
+      <c r="Z32" s="39">
         <v>11.6</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>1976</v>
       </c>
-      <c r="B33" s="37">
+      <c r="B33" s="53">
+        <v>14.9</v>
+      </c>
+      <c r="C33" s="40"/>
+      <c r="D33" s="37">
         <v>23.710999999999999</v>
       </c>
-      <c r="C33" s="38">
+      <c r="E33" s="38">
         <v>74.5</v>
       </c>
-      <c r="D33" s="39">
+      <c r="F33" s="39">
         <v>21.3</v>
       </c>
-      <c r="E33" s="39">
+      <c r="G33" s="39">
         <v>4.2</v>
       </c>
-      <c r="F33" s="39">
+      <c r="H33" s="39">
         <v>0</v>
       </c>
-      <c r="G33" s="40"/>
-      <c r="H33" s="39">
+      <c r="I33" s="40"/>
+      <c r="J33" s="39">
         <v>8.86</v>
       </c>
-      <c r="I33" s="39">
+      <c r="K33" s="39">
         <v>62.8</v>
       </c>
-      <c r="J33" s="39">
+      <c r="L33" s="39">
         <v>29.4</v>
       </c>
-      <c r="K33" s="39">
+      <c r="M33" s="39">
         <v>7.8</v>
       </c>
-      <c r="L33" s="39">
+      <c r="N33" s="39">
         <v>0</v>
       </c>
-      <c r="M33" s="40"/>
-      <c r="N33" s="39">
+      <c r="O33" s="40"/>
+      <c r="P33" s="39">
         <v>10.8</v>
       </c>
-      <c r="O33" s="39">
+      <c r="Q33" s="39">
         <v>57.3</v>
       </c>
-      <c r="P33" s="39">
+      <c r="R33" s="39">
         <v>33.6</v>
       </c>
-      <c r="Q33" s="39">
+      <c r="S33" s="39">
         <v>9.1</v>
       </c>
-      <c r="R33" s="39">
+      <c r="T33" s="39">
         <v>0</v>
       </c>
-      <c r="S33" s="40"/>
-      <c r="T33" s="39">
+      <c r="U33" s="40"/>
+      <c r="V33" s="39">
         <v>7.8760000000000003</v>
       </c>
-      <c r="U33" s="39">
+      <c r="W33" s="39">
         <v>61</v>
       </c>
-      <c r="V33" s="39">
+      <c r="X33" s="39">
         <v>20.9</v>
       </c>
-      <c r="W33" s="39">
+      <c r="Y33" s="39">
         <v>5.7</v>
       </c>
-      <c r="X33" s="39">
+      <c r="Z33" s="39">
         <v>12.4</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>1977</v>
       </c>
-      <c r="B34" s="37">
+      <c r="B34" s="53">
+        <v>13.9</v>
+      </c>
+      <c r="C34" s="40"/>
+      <c r="D34" s="37">
         <v>21.686</v>
       </c>
-      <c r="C34" s="38">
+      <c r="E34" s="38">
         <v>68.5</v>
       </c>
-      <c r="D34" s="39">
+      <c r="F34" s="39">
         <v>26.8</v>
       </c>
-      <c r="E34" s="39">
+      <c r="G34" s="39">
         <v>4.7</v>
       </c>
-      <c r="F34" s="39">
+      <c r="H34" s="39">
         <v>0</v>
       </c>
-      <c r="G34" s="40"/>
-      <c r="H34" s="39">
+      <c r="I34" s="40"/>
+      <c r="J34" s="39">
         <v>8.5619999999999994</v>
       </c>
-      <c r="I34" s="39">
+      <c r="K34" s="39">
         <v>61</v>
       </c>
-      <c r="J34" s="39">
+      <c r="L34" s="39">
         <v>30.5</v>
       </c>
-      <c r="K34" s="39">
+      <c r="M34" s="39">
         <v>8.5</v>
       </c>
-      <c r="L34" s="39">
+      <c r="N34" s="39">
         <v>0</v>
       </c>
-      <c r="M34" s="40"/>
-      <c r="N34" s="39">
+      <c r="O34" s="40"/>
+      <c r="P34" s="39">
         <v>12.46</v>
       </c>
-      <c r="O34" s="39">
+      <c r="Q34" s="39">
         <v>52.5</v>
       </c>
-      <c r="P34" s="39">
+      <c r="R34" s="39">
         <v>39.1</v>
       </c>
-      <c r="Q34" s="39">
+      <c r="S34" s="39">
         <v>8.4</v>
       </c>
-      <c r="R34" s="39">
+      <c r="T34" s="39">
         <v>0</v>
       </c>
-      <c r="S34" s="40"/>
-      <c r="T34" s="39">
+      <c r="U34" s="40"/>
+      <c r="V34" s="39">
         <v>7.2720000000000002</v>
       </c>
-      <c r="U34" s="39">
+      <c r="W34" s="39">
         <v>49.8</v>
       </c>
-      <c r="V34" s="39">
+      <c r="X34" s="39">
         <v>30.8</v>
       </c>
-      <c r="W34" s="39">
+      <c r="Y34" s="39">
         <v>5.7</v>
       </c>
-      <c r="X34" s="39">
+      <c r="Z34" s="39">
         <v>13.7</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>1978</v>
       </c>
-      <c r="B35" s="37">
+      <c r="B35" s="53">
+        <v>13.3</v>
+      </c>
+      <c r="C35" s="40"/>
+      <c r="D35" s="37">
         <v>20.614000000000001</v>
       </c>
-      <c r="C35" s="38">
+      <c r="E35" s="38">
         <v>68.8</v>
       </c>
-      <c r="D35" s="39">
+      <c r="F35" s="39">
         <v>27.1</v>
       </c>
-      <c r="E35" s="39">
+      <c r="G35" s="39">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F35" s="39">
+      <c r="H35" s="39">
         <v>0</v>
       </c>
-      <c r="G35" s="40"/>
-      <c r="H35" s="39">
+      <c r="I35" s="40"/>
+      <c r="J35" s="39">
         <v>7.593</v>
       </c>
-      <c r="I35" s="39">
+      <c r="K35" s="39">
         <v>50.8</v>
       </c>
-      <c r="J35" s="39">
+      <c r="L35" s="39">
         <v>39.4</v>
       </c>
-      <c r="K35" s="39">
+      <c r="M35" s="39">
         <v>9.6999999999999993</v>
       </c>
-      <c r="L35" s="39">
+      <c r="N35" s="39">
         <v>0</v>
       </c>
-      <c r="M35" s="40"/>
-      <c r="N35" s="39">
+      <c r="O35" s="40"/>
+      <c r="P35" s="39">
         <v>11.843</v>
       </c>
-      <c r="O35" s="39">
+      <c r="Q35" s="39">
         <v>52.8</v>
       </c>
-      <c r="P35" s="39">
+      <c r="R35" s="39">
         <v>38.799999999999997</v>
       </c>
-      <c r="Q35" s="39">
+      <c r="S35" s="39">
         <v>8.4</v>
       </c>
-      <c r="R35" s="39">
+      <c r="T35" s="39">
         <v>0</v>
       </c>
-      <c r="S35" s="40"/>
-      <c r="T35" s="39">
+      <c r="U35" s="40"/>
+      <c r="V35" s="39">
         <v>7.1989999999999998</v>
       </c>
-      <c r="U35" s="39">
+      <c r="W35" s="39">
         <v>47</v>
       </c>
-      <c r="V35" s="39">
+      <c r="X35" s="39">
         <v>33.5</v>
       </c>
-      <c r="W35" s="39">
-        <v>6</v>
-      </c>
-      <c r="X35" s="39">
+      <c r="Y35" s="39">
+        <v>6</v>
+      </c>
+      <c r="Z35" s="39">
         <v>13.5</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <v>1979</v>
       </c>
-      <c r="B36" s="39">
+      <c r="B36" s="53">
+        <v>12.8</v>
+      </c>
+      <c r="C36" s="40"/>
+      <c r="D36" s="39">
         <v>19.794</v>
       </c>
-      <c r="C36" s="38">
+      <c r="E36" s="38">
         <v>68.3</v>
       </c>
-      <c r="D36" s="39">
+      <c r="F36" s="39">
         <v>27.4</v>
       </c>
-      <c r="E36" s="39">
+      <c r="G36" s="39">
         <v>4.3</v>
       </c>
-      <c r="F36" s="39">
+      <c r="H36" s="39">
         <v>0</v>
       </c>
-      <c r="G36" s="40"/>
-      <c r="H36" s="39">
+      <c r="I36" s="40"/>
+      <c r="J36" s="39">
         <v>8.76</v>
       </c>
-      <c r="I36" s="39">
+      <c r="K36" s="39">
         <v>57.4</v>
       </c>
-      <c r="J36" s="39">
+      <c r="L36" s="39">
         <v>32.6</v>
       </c>
-      <c r="K36" s="39">
+      <c r="M36" s="39">
         <v>10</v>
       </c>
-      <c r="L36" s="39">
+      <c r="N36" s="39">
         <v>0</v>
       </c>
-      <c r="M36" s="40"/>
-      <c r="N36" s="39">
+      <c r="O36" s="40"/>
+      <c r="P36" s="39">
         <v>12.27</v>
       </c>
-      <c r="O36" s="39">
+      <c r="Q36" s="39">
         <v>53.5</v>
       </c>
-      <c r="P36" s="39">
+      <c r="R36" s="39">
         <v>37.5</v>
       </c>
-      <c r="Q36" s="39">
+      <c r="S36" s="39">
         <v>9</v>
       </c>
-      <c r="R36" s="39">
+      <c r="T36" s="39">
         <v>0</v>
       </c>
-      <c r="S36" s="40"/>
-      <c r="T36" s="39">
+      <c r="U36" s="40"/>
+      <c r="V36" s="39">
         <v>7.0709999999999997</v>
       </c>
-      <c r="U36" s="39">
+      <c r="W36" s="39">
         <v>50.6</v>
       </c>
-      <c r="V36" s="39">
+      <c r="X36" s="39">
         <v>41.6</v>
       </c>
-      <c r="W36" s="39">
+      <c r="Y36" s="39">
         <v>8</v>
       </c>
-      <c r="X36" s="39">
+      <c r="Z36" s="39">
         <v>15.6</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
         <v>1980</v>
       </c>
-      <c r="B37" s="39">
+      <c r="B37" s="53">
+        <v>11</v>
+      </c>
+      <c r="C37" s="40"/>
+      <c r="D37" s="39">
         <v>14.538</v>
       </c>
-      <c r="C37" s="38">
+      <c r="E37" s="38">
         <v>68.8</v>
       </c>
-      <c r="D37" s="39">
+      <c r="F37" s="39">
         <v>26.9</v>
       </c>
-      <c r="E37" s="39">
+      <c r="G37" s="39">
         <v>4.3</v>
       </c>
-      <c r="F37" s="39">
+      <c r="H37" s="39">
         <v>0</v>
       </c>
-      <c r="G37" s="40"/>
-      <c r="H37" s="39">
+      <c r="I37" s="40"/>
+      <c r="J37" s="39">
         <v>8.76</v>
       </c>
-      <c r="I37" s="39">
+      <c r="K37" s="39">
         <v>62</v>
       </c>
-      <c r="J37" s="39">
+      <c r="L37" s="39">
         <v>28.6</v>
       </c>
-      <c r="K37" s="39">
+      <c r="M37" s="39">
         <v>9.4</v>
       </c>
-      <c r="L37" s="39">
+      <c r="N37" s="39">
         <v>0</v>
       </c>
-      <c r="M37" s="40"/>
-      <c r="N37" s="39">
+      <c r="O37" s="40"/>
+      <c r="P37" s="39">
         <v>13.137</v>
       </c>
-      <c r="O37" s="39">
+      <c r="Q37" s="39">
         <v>50.1</v>
       </c>
-      <c r="P37" s="39">
+      <c r="R37" s="39">
         <v>40.799999999999997</v>
       </c>
-      <c r="Q37" s="39">
+      <c r="S37" s="39">
         <v>9.1</v>
       </c>
-      <c r="R37" s="39">
+      <c r="T37" s="39">
         <v>0</v>
       </c>
-      <c r="S37" s="40"/>
-      <c r="T37" s="39">
+      <c r="U37" s="40"/>
+      <c r="V37" s="39">
         <v>6.5789999999999997</v>
       </c>
-      <c r="U37" s="39">
+      <c r="W37" s="39">
         <v>41.9</v>
       </c>
-      <c r="V37" s="39">
+      <c r="X37" s="39">
         <v>37.799999999999997</v>
       </c>
-      <c r="W37" s="39">
+      <c r="Y37" s="39">
         <v>6.9</v>
       </c>
-      <c r="X37" s="39">
+      <c r="Z37" s="39">
         <v>13.3</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>1981</v>
       </c>
-      <c r="B38" s="39">
+      <c r="B38" s="53">
+        <v>12.3</v>
+      </c>
+      <c r="C38" s="40"/>
+      <c r="D38" s="39">
         <v>17.120999999999999</v>
       </c>
-      <c r="C38" s="38">
+      <c r="E38" s="38">
         <v>59</v>
       </c>
-      <c r="D38" s="39">
+      <c r="F38" s="39">
         <v>36.1</v>
       </c>
-      <c r="E38" s="39">
+      <c r="G38" s="39">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F38" s="39">
+      <c r="H38" s="39">
         <v>0</v>
       </c>
-      <c r="G38" s="40"/>
-      <c r="H38" s="39">
+      <c r="I38" s="40"/>
+      <c r="J38" s="39">
         <v>8.4280000000000008</v>
       </c>
-      <c r="I38" s="39">
+      <c r="K38" s="39">
         <v>52.1</v>
       </c>
-      <c r="J38" s="39">
+      <c r="L38" s="39">
         <v>38.6</v>
       </c>
-      <c r="K38" s="39">
+      <c r="M38" s="39">
         <v>9.3000000000000007</v>
       </c>
-      <c r="L38" s="39">
+      <c r="N38" s="39">
         <v>0</v>
       </c>
-      <c r="M38" s="40"/>
-      <c r="N38" s="39">
+      <c r="O38" s="40"/>
+      <c r="P38" s="39">
         <v>11.477</v>
       </c>
-      <c r="O38" s="39">
+      <c r="Q38" s="39">
         <v>48.9</v>
       </c>
-      <c r="P38" s="39">
+      <c r="R38" s="39">
         <v>41.6</v>
       </c>
-      <c r="Q38" s="39">
+      <c r="S38" s="39">
         <v>9.5</v>
       </c>
-      <c r="R38" s="39">
+      <c r="T38" s="39">
         <v>0</v>
       </c>
-      <c r="S38" s="40"/>
-      <c r="T38" s="39">
+      <c r="U38" s="40"/>
+      <c r="V38" s="39">
         <v>6.9930000000000003</v>
       </c>
-      <c r="U38" s="39">
+      <c r="W38" s="39">
         <v>43.3</v>
       </c>
-      <c r="V38" s="39">
+      <c r="X38" s="39">
         <v>36.4</v>
       </c>
-      <c r="W38" s="39">
+      <c r="Y38" s="39">
         <v>6.9</v>
       </c>
-      <c r="X38" s="39">
+      <c r="Z38" s="39">
         <v>13.4</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
         <v>1982</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="11">
         <v>1983</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
         <v>1984</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="11">
         <v>1985</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
         <v>1986</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="11">
         <v>1987</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
         <v>1988</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
         <v>1989</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
         <v>1990</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
         <v>1991</v>
       </c>
@@ -13873,62 +14002,66 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
         <v>2008</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="11">
         <v>2009</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="11">
         <v>2010</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="11">
         <v>2011</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B68" s="51">
+        <f>6.1+0.8+2.1</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="11">
         <v>2012</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="11">
         <v>2013</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="11">
         <v>2014</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="11">
         <v>2015</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="11">
         <v>2016</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="11">
         <v>2017</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="11">
         <v>2018</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="11">
         <v>2019</v>
       </c>

</xml_diff>

<commit_message>
A new notebook specifically dedicated to IGU. Idem for RawData
</commit_message>
<xml_diff>
--- a/RawData/EU_RawData_VPython.xlsx
+++ b/RawData/EU_RawData_VPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\01_MFA_GlassIndustry\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6704EDD0-2573-48B4-AA28-6363BD0CF4B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112A9C13-01CF-4B9D-AA78-788CCA29F668}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="2" xr2:uid="{123E2ECC-8474-4F38-AC8E-530CCC4039F8}"/>
   </bookViews>
@@ -5184,10 +5184,10 @@
   <dimension ref="A1:BT102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J75" sqref="J75"/>
+      <selection pane="bottomRight" activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>